<commit_message>
Updated documentation for milestone submission.
</commit_message>
<xml_diff>
--- a/Planning and Design/CST-247-RS-SprintBurnDown - CLC.xlsx
+++ b/Planning and Design/CST-247-RS-SprintBurnDown - CLC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Documents\Grand Canyon University\Classes\CST-247\CLC - Week 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cameron\Documents\Grand Canyon University\Classes\CST-247\CLC - Week 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18330" windowHeight="9075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Burn Down Chart" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Task</t>
   </si>
@@ -135,48 +135,36 @@
     <t>After each Daily Standup each Team Member should review the Burn Down Chart to ensure your Sprint will be delivered on time</t>
   </si>
   <si>
-    <t>As a(n) user create an account with the website.</t>
-  </si>
-  <si>
     <t>Vinson Martin</t>
   </si>
   <si>
-    <t>Registration page/view</t>
-  </si>
-  <si>
-    <t>As a(n) user login to the web application</t>
-  </si>
-  <si>
-    <t>Login page/view</t>
-  </si>
-  <si>
-    <t>As a(n) developer control the login information.</t>
-  </si>
-  <si>
-    <t>Login controller</t>
-  </si>
-  <si>
     <t>Cameron Deao</t>
   </si>
   <si>
-    <t>As a(n) developer control the registration information being passed by the views.</t>
-  </si>
-  <si>
-    <t>As a(n) store user information.</t>
-  </si>
-  <si>
-    <t>SQL Database</t>
-  </si>
-  <si>
     <t>Joseph Cooper</t>
   </si>
   <si>
-    <t>Registration controller</t>
-  </si>
-  <si>
     <t>Project Title: Minsweeper Web Application
-Release #: 0.1
-Sprint #: 1</t>
+Release #: 0.3
+Sprint #: 3</t>
+  </si>
+  <si>
+    <t>Game board logic</t>
+  </si>
+  <si>
+    <t>As a(n) developer, I would like to create the logic for gameplay.</t>
+  </si>
+  <si>
+    <t>As a(n) developer, I would like to showcase a 12x12 game grid of Minesweeper.</t>
+  </si>
+  <si>
+    <t>As a(n) user, I would like to view a home page after logging in to the application</t>
+  </si>
+  <si>
+    <t>Home page/view</t>
+  </si>
+  <si>
+    <t>Game board view and controller</t>
   </si>
 </sst>
 </file>
@@ -363,10 +351,96 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:idx val="2"/>
+          <c:order val="2"/>
           <c:tx>
-            <c:v>Ideal burndown</c:v>
+            <c:v>Ideal</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burn Down Chart'!$F$14:$P$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.599999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12.999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10.399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.7999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.1999999999999975</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5999999999999974</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Actual</c:v>
           </c:tx>
           <c:dLbls>
             <c:spPr>
@@ -386,189 +460,47 @@
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
-                <c15:showLeaderLines val="0"/>
+                <c15:showLeaderLines val="1"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]Sheet1!$F$5:$O$5</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
+          <c:val>
+            <c:numRef>
+              <c:f>'Burn Down Chart'!$F$15:$P$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>Day 10</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Day 9</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Day 8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Day 2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]Sheet1!$F$19:$O$19</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Actual burndown</c:v>
-          </c:tx>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="0"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>[1]Sheet1!$F$5:$O$5</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Day 10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Day 2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>[1]Sheet1!$F$20:$O$20</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -586,11 +518,255 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="411988944"/>
-        <c:axId val="411976792"/>
+        <c:axId val="466029448"/>
+        <c:axId val="466030624"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>Ideal burndown</c:v>
+                </c:tx>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="0"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet1!$F$5:$O$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>Day 10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Day 9</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Day 8</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Day 7</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Day 6</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Day 5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Day 4</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Day 3</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Day 2</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>Day 1</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet1!$F$19:$O$19</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>12</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>9</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>Actual burndown</c:v>
+                </c:tx>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="0"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet1!$F$5:$O$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>Day 10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Day 9</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>Day 8</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>Day 7</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>Day 6</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>Day 5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>Day 4</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>Day 3</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>Day 2</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>Day 1</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet1!$F$20:$O$20</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="10"/>
+                      <c:pt idx="0">
+                        <c:v>29</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>27</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>21</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>17</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>11</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>6</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="411988944"/>
+        <c:axId val="466029448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,7 +776,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="411976792"/>
+        <c:crossAx val="466030624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -608,7 +784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="411976792"/>
+        <c:axId val="466030624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,7 +794,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="411988944"/>
+        <c:crossAx val="466029448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1056,8 +1232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="X15" sqref="X15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,7 +1246,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1149,43 +1325,43 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="7">
         <v>1</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>35</v>
       </c>
       <c r="F4" s="4">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
         <v>2</v>
       </c>
-      <c r="G4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0</v>
-      </c>
       <c r="J4" s="4">
         <v>0</v>
       </c>
       <c r="K4" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L4" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M4" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N4" s="4">
         <v>0</v>
@@ -1205,7 +1381,9 @@
       <c r="C5" s="10"/>
       <c r="D5" s="9"/>
       <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
       <c r="G5" s="4">
         <v>0</v>
       </c>
@@ -1317,22 +1495,22 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="7">
         <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="4">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -1341,16 +1519,16 @@
         <v>0</v>
       </c>
       <c r="I8" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J8" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K8" s="4">
         <v>0</v>
       </c>
       <c r="L8" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M8" s="4">
         <v>0</v>
@@ -1451,22 +1629,22 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="7">
         <v>3</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="F11" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11" s="4">
         <v>0</v>
@@ -1475,7 +1653,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J11" s="4">
         <v>0</v>
@@ -1501,23 +1679,15 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="7">
         <v>4</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="4">
-        <v>3</v>
-      </c>
+      <c r="C12" s="10"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="4">
         <v>0</v>
       </c>
@@ -1551,23 +1721,15 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="7">
         <v>5</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="4">
-        <v>4</v>
-      </c>
+      <c r="C13" s="10"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="4">
         <v>0</v>
       </c>
@@ -1611,47 +1773,47 @@
       <c r="E14" s="12"/>
       <c r="F14" s="4">
         <f>SUM(F4:F13)</f>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G14" s="4">
         <f>F14-$F$14/10</f>
-        <v>12.6</v>
+        <v>23.4</v>
       </c>
       <c r="H14" s="4">
-        <f t="shared" ref="H14:P14" si="0">G14-$F$14/10</f>
-        <v>11.2</v>
+        <f t="shared" ref="H14:O14" si="0">G14-$F$14/10</f>
+        <v>20.799999999999997</v>
       </c>
       <c r="I14" s="4">
         <f t="shared" si="0"/>
-        <v>9.7999999999999989</v>
+        <v>18.199999999999996</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="0"/>
-        <v>8.3999999999999986</v>
+        <v>15.599999999999996</v>
       </c>
       <c r="K14" s="4">
         <f t="shared" si="0"/>
-        <v>6.9999999999999982</v>
+        <v>12.999999999999996</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" si="0"/>
-        <v>5.5999999999999979</v>
+        <v>10.399999999999997</v>
       </c>
       <c r="M14" s="4">
         <f t="shared" si="0"/>
-        <v>4.1999999999999975</v>
+        <v>7.7999999999999972</v>
       </c>
       <c r="N14" s="4">
         <f t="shared" si="0"/>
-        <v>2.7999999999999976</v>
+        <v>5.1999999999999975</v>
       </c>
       <c r="O14" s="4">
         <f t="shared" si="0"/>
-        <v>1.3999999999999977</v>
+        <v>2.5999999999999974</v>
       </c>
       <c r="P14" s="4">
-        <f t="shared" si="0"/>
-        <v>-2.2204460492503131E-15</v>
+        <f>O14-$F$14/10</f>
+        <v>0</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -1666,19 +1828,19 @@
       <c r="E15" s="12"/>
       <c r="F15" s="4">
         <f>SUM(F4:F13)</f>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" ref="G15:P15" si="1">F15 - SUM(G4:G13)</f>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="I15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="1"/>
@@ -1686,27 +1848,27 @@
       </c>
       <c r="K15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="M15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="O15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="P15" s="4">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -2507,21 +2669,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2544,14 +2706,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D6E300D-687F-49DD-9C99-AC5EA1BE3BF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C1BE12-9AF4-4D82-8933-6D42A4A8E2C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2566,4 +2720,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D6E300D-687F-49DD-9C99-AC5EA1BE3BF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>